<commit_message>
Just started tagging images. Need to connect to database, retrieve information, and start using it.
</commit_message>
<xml_diff>
--- a/example-files/photoshoot.xlsx
+++ b/example-files/photoshoot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\nate\code\awim\example-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8577143F-754D-4161-9CED-78BCA45D397C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD79FC6-8780-41D0-AE2C-09F9CDB2F4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="6345" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -279,15 +279,10 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -300,6 +295,11 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,7 +586,7 @@
   <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="H23" sqref="H23:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,17 +626,17 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
       <c r="N1" s="5"/>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="13" t="s">
+      <c r="P1" s="19"/>
+      <c r="Q1" s="11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="9"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -664,22 +664,22 @@
       <c r="K2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="19" t="s">
+      <c r="Q2" s="16" t="s">
         <v>47</v>
       </c>
     </row>
@@ -687,7 +687,7 @@
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="6">
@@ -717,7 +717,7 @@
         <f t="shared" ref="J3:J21" si="4">I3+$C$24</f>
         <v>38</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="17">
         <v>542</v>
       </c>
       <c r="L3" s="6">
@@ -727,22 +727,22 @@
       <c r="M3" s="6">
         <v>3</v>
       </c>
-      <c r="N3" s="18">
+      <c r="N3" s="15">
         <v>53</v>
       </c>
-      <c r="O3" s="18">
+      <c r="O3" s="15">
         <v>26</v>
       </c>
-      <c r="P3" s="18">
+      <c r="P3" s="15">
         <v>55</v>
       </c>
-      <c r="Q3" s="14"/>
+      <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="6">
@@ -772,7 +772,7 @@
         <f t="shared" si="4"/>
         <v>38</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="17">
         <v>457</v>
       </c>
       <c r="L4" s="6">
@@ -782,22 +782,22 @@
       <c r="M4" s="6">
         <v>10</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N4" s="15">
         <v>53</v>
       </c>
-      <c r="O4" s="18">
+      <c r="O4" s="15">
         <v>146</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P4" s="15">
         <v>159</v>
       </c>
-      <c r="Q4" s="14"/>
+      <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="15" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="6">
@@ -827,7 +827,7 @@
         <f t="shared" si="4"/>
         <v>38</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="17">
         <v>453</v>
       </c>
       <c r="L5" s="6">
@@ -837,22 +837,22 @@
       <c r="M5" s="6">
         <v>21</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="15">
         <v>102</v>
       </c>
-      <c r="O5" s="18">
+      <c r="O5" s="15">
         <v>114</v>
       </c>
-      <c r="P5" s="18">
+      <c r="P5" s="15">
         <v>145</v>
       </c>
-      <c r="Q5" s="14"/>
+      <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="6">
@@ -882,7 +882,7 @@
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="17">
         <v>506</v>
       </c>
       <c r="L6" s="6">
@@ -892,22 +892,22 @@
       <c r="M6" s="6">
         <v>40</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="15">
         <v>143</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="15">
         <v>146</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="15">
         <v>123</v>
       </c>
-      <c r="Q6" s="14"/>
+      <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="6">
@@ -938,7 +938,7 @@
         <f t="shared" si="4"/>
         <v>78</v>
       </c>
-      <c r="K7" s="20">
+      <c r="K7" s="17">
         <v>456</v>
       </c>
       <c r="L7" s="6">
@@ -948,22 +948,22 @@
       <c r="M7" s="6">
         <v>47</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="15">
         <v>143</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="15">
         <v>107</v>
       </c>
-      <c r="P7" s="20">
+      <c r="P7" s="17">
         <v>146</v>
       </c>
-      <c r="Q7" s="14"/>
+      <c r="Q7" s="12"/>
     </row>
     <row r="8" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="6">
@@ -993,7 +993,7 @@
         <f t="shared" si="4"/>
         <v>98</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8" s="17">
         <v>543</v>
       </c>
       <c r="L8" s="6">
@@ -1002,22 +1002,22 @@
       <c r="M8" s="6">
         <v>85</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="15">
         <v>233</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="15">
         <v>0</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="15">
         <v>0</v>
       </c>
-      <c r="Q8" s="14"/>
+      <c r="Q8" s="12"/>
     </row>
     <row r="9" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="6">
@@ -1047,7 +1047,7 @@
         <f t="shared" si="4"/>
         <v>38</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9" s="17">
         <v>549</v>
       </c>
       <c r="L9" s="6">
@@ -1057,22 +1057,22 @@
       <c r="M9" s="6">
         <v>24</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="15">
         <v>174</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="15">
         <v>48</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="15">
         <v>31</v>
       </c>
-      <c r="Q9" s="14"/>
+      <c r="Q9" s="12"/>
     </row>
     <row r="10" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="6">
@@ -1102,7 +1102,7 @@
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="17">
         <v>550</v>
       </c>
       <c r="L10" s="6">
@@ -1112,22 +1112,22 @@
       <c r="M10" s="6">
         <v>21</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="15">
         <v>174</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10" s="15">
         <v>32</v>
       </c>
-      <c r="P10" s="18">
+      <c r="P10" s="15">
         <v>-3</v>
       </c>
-      <c r="Q10" s="14"/>
+      <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="6">
@@ -1157,21 +1157,21 @@
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K11" s="17">
         <v>552</v>
       </c>
-      <c r="L11" s="20">
+      <c r="L11" s="17">
         <v>234</v>
       </c>
-      <c r="M11" s="20">
+      <c r="M11" s="17">
         <v>14</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="15">
         <v>240</v>
       </c>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="21" t="s">
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="18" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
       <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="6">
@@ -1209,7 +1209,7 @@
         <f t="shared" si="4"/>
         <v>38</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12" s="17">
         <v>531</v>
       </c>
       <c r="L12" s="6">
@@ -1219,22 +1219,22 @@
       <c r="M12" s="6">
         <v>10</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="15">
         <v>233</v>
       </c>
-      <c r="O12" s="18">
+      <c r="O12" s="15">
         <v>139</v>
       </c>
-      <c r="P12" s="18">
+      <c r="P12" s="15">
         <v>174</v>
       </c>
-      <c r="Q12" s="14"/>
+      <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="6">
@@ -1264,7 +1264,7 @@
         <f t="shared" si="4"/>
         <v>38</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K13" s="17">
         <v>541</v>
       </c>
       <c r="L13" s="6">
@@ -1274,22 +1274,22 @@
       <c r="M13" s="6">
         <v>12</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="15">
         <v>270</v>
       </c>
-      <c r="O13" s="18">
+      <c r="O13" s="15">
         <v>71</v>
       </c>
-      <c r="P13" s="18">
+      <c r="P13" s="15">
         <v>110</v>
       </c>
-      <c r="Q13" s="14"/>
+      <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="6">
@@ -1319,7 +1319,7 @@
         <f t="shared" si="4"/>
         <v>38</v>
       </c>
-      <c r="K14" s="20">
+      <c r="K14" s="17">
         <v>540</v>
       </c>
       <c r="L14" s="6">
@@ -1329,22 +1329,22 @@
       <c r="M14" s="6">
         <v>9</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="15">
         <v>270</v>
       </c>
-      <c r="O14" s="18">
+      <c r="O14" s="15">
         <v>126</v>
       </c>
-      <c r="P14" s="18">
+      <c r="P14" s="15">
         <v>110</v>
       </c>
-      <c r="Q14" s="14"/>
+      <c r="Q14" s="12"/>
     </row>
     <row r="15" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="6">
@@ -1374,22 +1374,22 @@
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="K15" s="20">
+      <c r="K15" s="17">
         <v>553</v>
       </c>
-      <c r="L15" s="20">
+      <c r="L15" s="17">
         <v>196</v>
       </c>
-      <c r="M15" s="20">
+      <c r="M15" s="17">
         <v>28</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="15">
         <f>270-34</f>
         <v>236</v>
       </c>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="21" t="s">
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="18" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="6">
@@ -1427,7 +1427,7 @@
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="K16" s="20">
+      <c r="K16" s="17">
         <v>537</v>
       </c>
       <c r="L16" s="6">
@@ -1437,22 +1437,22 @@
       <c r="M16" s="6">
         <v>38</v>
       </c>
-      <c r="N16" s="18">
+      <c r="N16" s="15">
         <v>323</v>
       </c>
-      <c r="O16" s="18">
+      <c r="O16" s="15">
         <v>104</v>
       </c>
-      <c r="P16" s="18">
+      <c r="P16" s="15">
         <v>141</v>
       </c>
-      <c r="Q16" s="14"/>
+      <c r="Q16" s="12"/>
     </row>
     <row r="17" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="6">
@@ -1488,13 +1488,13 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
-      <c r="Q17" s="14"/>
+      <c r="Q17" s="12"/>
     </row>
     <row r="18" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="6">
@@ -1530,13 +1530,13 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-      <c r="Q18" s="14"/>
+      <c r="Q18" s="12"/>
     </row>
     <row r="19" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="6">
@@ -1572,13 +1572,13 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-      <c r="Q19" s="14"/>
+      <c r="Q19" s="12"/>
     </row>
     <row r="20" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="6">
@@ -1614,13 +1614,13 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
-      <c r="Q20" s="14"/>
+      <c r="Q20" s="12"/>
     </row>
     <row r="21" spans="1:17" ht="21" x14ac:dyDescent="0.5">
       <c r="A21" s="5">
         <v>19</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C21" s="6">
@@ -1656,13 +1656,13 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
-      <c r="Q21" s="14"/>
+      <c r="Q21" s="12"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="20">
         <v>43</v>
       </c>
       <c r="D23" s="4"/>
@@ -1671,7 +1671,7 @@
       <c r="G23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="20">
         <f>360-37</f>
         <v>323</v>
       </c>
@@ -1680,7 +1680,7 @@
       <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="20">
         <v>28</v>
       </c>
       <c r="D24" s="4"/>
@@ -1689,7 +1689,7 @@
       <c r="G24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="20">
         <f>90-37</f>
         <v>53</v>
       </c>
@@ -1698,7 +1698,7 @@
       <c r="B25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="4"/>
@@ -1707,7 +1707,7 @@
       <c r="G25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="20">
         <f>180-37</f>
         <v>143</v>
       </c>
@@ -1716,7 +1716,7 @@
       <c r="B26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="4"/>
@@ -1725,7 +1725,7 @@
       <c r="G26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="20">
         <f>270-37</f>
         <v>233</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="4"/>
@@ -1747,7 +1747,7 @@
       <c r="B28" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="20" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="4"/>

</xml_diff>